<commit_message>
add search chat function
</commit_message>
<xml_diff>
--- a/Bao cao tu danh gia.xlsx
+++ b/Bao cao tu danh gia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\IdeaProjects\Chat-System\Chat-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA090D5E-618D-46ED-9D81-8EC36BCDE869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8116DDB-2204-41A3-AEBB-1E7A3B1B97FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1018,8 +1018,8 @@
   <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="I1" s="14">
         <f>MAX(10+SUM(F2:F68), 0)</f>
-        <v>7.8250000000000002</v>
+        <v>8.5749999999999993</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -2162,11 +2162,11 @@
         <v>78</v>
       </c>
       <c r="E59" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F59" s="5">
         <f t="shared" si="10"/>
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2183,11 +2183,11 @@
         <v>78</v>
       </c>
       <c r="E60" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60" s="5">
         <f t="shared" si="10"/>
-        <v>-0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update system and report
</commit_message>
<xml_diff>
--- a/Bao cao tu danh gia.xlsx
+++ b/Bao cao tu danh gia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\IdeaProjects\Chat-System\Chat-System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\3rd year - 1st sem\java\project\Chat-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8116DDB-2204-41A3-AEBB-1E7A3B1B97FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4F9BBA-9FEC-42D2-9085-36E3A65C464D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thong tin nhom" sheetId="6" r:id="rId1"/>
@@ -908,16 +908,16 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" customWidth="1"/>
-    <col min="2" max="2" width="26.59765625" customWidth="1"/>
-    <col min="3" max="3" width="26.8984375" customWidth="1"/>
-    <col min="4" max="4" width="29.3984375" customWidth="1"/>
-    <col min="5" max="5" width="29.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="26.625" customWidth="1"/>
+    <col min="3" max="3" width="26.875" customWidth="1"/>
+    <col min="4" max="4" width="29.375" customWidth="1"/>
+    <col min="5" max="5" width="29.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>6</v>
       </c>
@@ -925,7 +925,7 @@
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
@@ -939,19 +939,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>11</v>
       </c>
@@ -959,7 +959,7 @@
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
@@ -976,28 +976,28 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1017,23 +1017,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.09765625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="44.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="44.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="1"/>
-    <col min="4" max="4" width="31.3984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.3984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.375" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1057,10 +1057,10 @@
       </c>
       <c r="I1" s="14">
         <f>MAX(10+SUM(F2:F68), 0)</f>
-        <v>8.5749999999999993</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>8.0250000000000004</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="13" t="s">
         <v>17</v>
@@ -1073,7 +1073,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -1085,7 +1085,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>1.1000000000000001</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>-4.9999999999999989E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>1.2</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>-0.19999999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>1.3</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>1.4</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>-4.9999999999999989E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>1.5</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>1.6</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>1.7</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>2</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>-9.9999999999999978E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>3</v>
       </c>
@@ -1265,7 +1265,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>3.1</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>-4.9999999999999989E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>3.2</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>3.3</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>3.4</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>4</v>
       </c>
@@ -1361,7 +1361,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>4.0999999999999996</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>-4.9999999999999989E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>4.2</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>-4.9999999999999989E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>4.3</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>5</v>
       </c>
@@ -1436,7 +1436,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>5.0999999999999996</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>-4.9999999999999989E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>5.2</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>-0.125</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>6</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>7</v>
       </c>
@@ -1511,7 +1511,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>7.1</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>-4.9999999999999989E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>7.2</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>7.3</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>8</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>8.1</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>-4.9999999999999989E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>8.1999999999999993</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>8.3000000000000007</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>9</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
       <c r="B34" s="20" t="s">
         <v>44</v>
@@ -1680,7 +1680,7 @@
       <c r="E34" s="7"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>1</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>2</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>3</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>4</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>5</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>6</v>
       </c>
@@ -1797,7 +1797,7 @@
       <c r="E40" s="7"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>6.1</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>6.2</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>6.3</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>-4.9999999999999989E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>6.4</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>7</v>
       </c>
@@ -1893,7 +1893,7 @@
       <c r="E45" s="7"/>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>7.1</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>7.2</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <v>8</v>
       </c>
@@ -1947,7 +1947,7 @@
       <c r="E48" s="7"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <v>8.1</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <v>8.1999999999999993</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>-9.9999999999999978E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <v>9</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <v>10</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <v>11</v>
       </c>
@@ -2043,7 +2043,7 @@
       <c r="E53" s="7"/>
       <c r="F53" s="5"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <v>11.1</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <v>11.2</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>-9.9999999999999978E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <v>11.3</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <v>11.4</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <v>11.5</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <v>11.6</v>
       </c>
@@ -2162,14 +2162,14 @@
         <v>78</v>
       </c>
       <c r="E59" s="6">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F59" s="5">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-4.9999999999999989E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <v>11.7</v>
       </c>
@@ -2183,14 +2183,14 @@
         <v>78</v>
       </c>
       <c r="E60" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F60" s="5">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <v>12</v>
       </c>
@@ -2202,7 +2202,7 @@
       <c r="E61" s="7"/>
       <c r="F61" s="5"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <v>12.1</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <v>12.2</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <v>12.3</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>-4.9999999999999989E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <v>12.4</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <v>12.5</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>-4.9999999999999989E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <v>12.6</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <v>12.7</v>
       </c>

</xml_diff>